<commit_message>
img, exccel, erros w3c
</commit_message>
<xml_diff>
--- a/P4_01_analyse.xlsx
+++ b/P4_01_analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Openclassrooms\Projets\P4_phlippoteau_quentin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2290EB0-113C-481E-850F-971FA563BEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C803E1-5100-4849-BA9A-7C5F254B8D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analyse" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="178">
   <si>
     <t>Catégorie</t>
   </si>
@@ -1552,9 +1552,6 @@
     <t>le type permet filtrer les réponses des utilisateurs. Pour une question ouverte, je recommande "text"</t>
   </si>
   <si>
-    <t>&lt;input class="form-control" type="text" required id="input_504" /&gt;</t>
-  </si>
-  <si>
     <t>&lt;form id="form_1" novalidate success-msg="Your message has been sent." fail-msg="Sorry it seems that our mail server is not responding, Sorry for the inconvenience!"&gt;</t>
   </si>
   <si>
@@ -1771,9 +1768,6 @@
 					&lt;p class="auteur"&gt; Maxime Guibard, PDG À vos fourchettes&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;link rel="stylesheet" type="text/css" href="./css/bootstrap.css"&gt;</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1834,6 +1828,123 @@
   <si>
     <t>erreur W3C :
 Error: Attribute success-msg not allowed on element form at this point.</t>
+  </si>
+  <si>
+    <t>erreur W3C :
+le ID ne peut être utilisé qu'une seule fois</t>
+  </si>
+  <si>
+    <t>Utiliser des classes plutôt qu'un ID si on doit réutilisser cette div</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;a href="contact.html" class="btn btn-lg btn-clean btn-rd </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>cta-hero</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="3" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> btn-atomic-black"&gt;Contact&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;form id="form_1" novalidate&gt;</t>
+  </si>
+  <si>
+    <t>Supprimer les erreurs signalés par le W3C</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="3" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;input class="form-control" type=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="3" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> required id="input_504" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;link rel="stylesheet" type="text/css" href="./css/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bootstrap.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="3" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="page2.html" class="btn btn-lg btn-clean btn-rd cta-hero btn-atomic-tangerine" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>id="cta-hero"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;Contact&lt;/a&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2089,7 +2200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2228,6 +2339,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2240,26 +2360,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2484,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2542,7 +2665,7 @@
     </row>
     <row r="2" spans="1:26" ht="104.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>132</v>
@@ -2563,7 +2686,7 @@
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="103.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>10</v>
@@ -2584,7 +2707,7 @@
     </row>
     <row r="4" spans="1:26" ht="182.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>15</v>
@@ -2604,10 +2727,10 @@
       <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:26" s="13" customFormat="1" ht="182.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="57" t="s">
+      <c r="A5" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>103</v>
       </c>
       <c r="C5" s="35" t="s">
@@ -2616,7 +2739,7 @@
       <c r="D5" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="50" t="s">
         <v>104</v>
       </c>
       <c r="F5" s="36" t="s">
@@ -2626,7 +2749,7 @@
     </row>
     <row r="6" spans="1:26" s="7" customFormat="1" ht="86.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>17</v>
@@ -2647,7 +2770,7 @@
     </row>
     <row r="7" spans="1:26" ht="97.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>138</v>
@@ -2668,7 +2791,7 @@
     </row>
     <row r="8" spans="1:26" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>26</v>
@@ -2689,7 +2812,7 @@
     </row>
     <row r="9" spans="1:26" ht="126.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>73</v>
@@ -2710,7 +2833,7 @@
     </row>
     <row r="10" spans="1:26" ht="115.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>76</v>
@@ -2730,16 +2853,16 @@
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:26" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
-        <v>156</v>
+      <c r="A11" s="51" t="s">
+        <v>155</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="53" t="s">
         <v>125</v>
       </c>
       <c r="E11" s="23" t="s">
@@ -2751,25 +2874,25 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:26" ht="124.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F12" s="33"/>
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:26" ht="86.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="31" t="s">
         <v>81</v>
       </c>
@@ -2778,15 +2901,15 @@
     </row>
     <row r="14" spans="1:26" s="8" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="49"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="9" t="s">
         <v>127</v>
       </c>
@@ -2795,15 +2918,15 @@
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="26" t="s">
         <v>108</v>
       </c>
@@ -2812,7 +2935,7 @@
     </row>
     <row r="16" spans="1:26" s="13" customFormat="1" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B16" s="35" t="s">
         <v>99</v>
@@ -2832,16 +2955,16 @@
       <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
-        <v>156</v>
+      <c r="A17" s="51" t="s">
+        <v>155</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="53" t="s">
         <v>123</v>
       </c>
       <c r="E17" s="22" t="s">
@@ -2851,12 +2974,12 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="37" t="s">
         <v>120</v>
       </c>
@@ -2864,12 +2987,12 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="37" t="s">
         <v>121</v>
       </c>
@@ -2877,12 +3000,12 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="37" t="s">
         <v>122</v>
       </c>
@@ -2890,22 +3013,22 @@
       <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
+      <c r="A21" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>19</v>
@@ -2914,14 +3037,14 @@
         <v>20</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>134</v>
@@ -2942,27 +3065,27 @@
     </row>
     <row r="24" spans="1:7" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C24" s="35" t="s">
         <v>139</v>
       </c>
       <c r="D24" s="38"/>
-      <c r="E24" s="35" t="s">
-        <v>168</v>
+      <c r="E24" s="61" t="s">
+        <v>176</v>
       </c>
       <c r="F24" s="38"/>
       <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:7" s="13" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C25" s="35" t="s">
         <v>147</v>
@@ -2971,28 +3094,51 @@
         <v>148</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:7" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
+        <v>169</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="60" t="s">
+        <v>173</v>
+      </c>
       <c r="F26" s="38"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" s="62"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="59"/>
+    </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3968,6 +4114,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="C14:D14"/>
@@ -3976,7 +4123,6 @@
     <mergeCell ref="D17:D20"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
-    <mergeCell ref="A21:F21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{8EA332A2-B751-44F4-BBB2-8AFA5734B8C1}"/>
@@ -4001,7 +4147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6AF312-AF06-4109-A2D8-7F9D6CA5465E}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -4014,13 +4160,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>160</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4036,7 +4182,7 @@
     </row>
     <row r="3" spans="1:3" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="42" t="s">
         <v>83</v>
@@ -4083,7 +4229,7 @@
         <v>98</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="46" t="s">
         <v>131</v>
@@ -4118,7 +4264,7 @@
       <c r="B10" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="58" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4129,7 +4275,7 @@
       <c r="B11" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="52"/>
+      <c r="C11" s="58"/>
     </row>
     <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
@@ -4138,25 +4284,25 @@
       <c r="B12" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="58"/>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="C13" s="46" t="s">
         <v>165</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="45" t="s">
         <v>151</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>152</v>
       </c>
       <c r="C14" s="47"/>
     </row>

</xml_diff>